<commit_message>
Minor changes with the addition of a couple files including Control Panel and Harness Diagram.
</commit_message>
<xml_diff>
--- a/Wire Harness/Connector Netlist.xlsx
+++ b/Wire Harness/Connector Netlist.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franklin.320\Buckeye Current\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235" tabRatio="500"/>
+    <workbookView xWindow="8840" yWindow="0" windowWidth="25520" windowHeight="15580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="57">
   <si>
     <t>Connector</t>
   </si>
@@ -181,9 +176,6 @@
     <t>-</t>
   </si>
   <si>
-    <t xml:space="preserve">+9-13.2V </t>
-  </si>
-  <si>
     <t>+12V AUX</t>
   </si>
   <si>
@@ -206,6 +198,9 @@
   </si>
   <si>
     <t>Pin #</t>
+  </si>
+  <si>
+    <t>12V AUX</t>
   </si>
 </sst>
 </file>
@@ -655,29 +650,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="11" style="6"/>
-    <col min="2" max="2" width="6.25" style="4" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="18.75">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -688,7 +683,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -699,7 +694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -710,7 +705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -721,7 +716,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
@@ -732,7 +727,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
@@ -743,7 +738,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="6" t="s">
         <v>5</v>
       </c>
@@ -754,7 +749,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
@@ -765,7 +760,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="6" t="s">
         <v>5</v>
       </c>
@@ -776,7 +771,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="6" t="s">
         <v>5</v>
       </c>
@@ -787,7 +782,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="6" t="s">
         <v>6</v>
       </c>
@@ -798,7 +793,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="6" t="s">
         <v>6</v>
       </c>
@@ -809,7 +804,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="6" t="s">
         <v>6</v>
       </c>
@@ -820,7 +815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" s="6" t="s">
         <v>6</v>
       </c>
@@ -831,7 +826,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" s="6" t="s">
         <v>6</v>
       </c>
@@ -842,7 +837,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3">
       <c r="A20" s="6" t="s">
         <v>7</v>
       </c>
@@ -853,7 +848,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3">
       <c r="A21" s="6" t="s">
         <v>7</v>
       </c>
@@ -864,7 +859,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3">
       <c r="A23" s="6" t="s">
         <v>8</v>
       </c>
@@ -875,7 +870,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3">
       <c r="A24" s="6" t="s">
         <v>8</v>
       </c>
@@ -886,7 +881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" s="6" t="s">
         <v>8</v>
       </c>
@@ -897,7 +892,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" s="6" t="s">
         <v>8</v>
       </c>
@@ -908,7 +903,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" s="6" t="s">
         <v>8</v>
       </c>
@@ -919,7 +914,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" s="6" t="s">
         <v>10</v>
       </c>
@@ -930,7 +925,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" s="6" t="s">
         <v>10</v>
       </c>
@@ -941,7 +936,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3">
       <c r="A31" s="6" t="s">
         <v>10</v>
       </c>
@@ -952,7 +947,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3">
       <c r="A32" s="6" t="s">
         <v>10</v>
       </c>
@@ -963,7 +958,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3">
       <c r="A33" s="6" t="s">
         <v>10</v>
       </c>
@@ -974,7 +969,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3">
       <c r="A35" s="6" t="s">
         <v>11</v>
       </c>
@@ -985,7 +980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" s="6" t="s">
         <v>11</v>
       </c>
@@ -996,7 +991,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" s="6" t="s">
         <v>12</v>
       </c>
@@ -1007,7 +1002,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" s="6" t="s">
         <v>12</v>
       </c>
@@ -1018,7 +1013,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" s="6" t="s">
         <v>15</v>
       </c>
@@ -1029,7 +1024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3">
       <c r="A42" s="6" t="s">
         <v>15</v>
       </c>
@@ -1040,7 +1035,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3">
       <c r="A44" s="6" t="s">
         <v>16</v>
       </c>
@@ -1051,7 +1046,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3">
       <c r="A45" s="6" t="s">
         <v>16</v>
       </c>
@@ -1062,7 +1057,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" s="6" t="s">
         <v>17</v>
       </c>
@@ -1073,7 +1068,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" s="6" t="s">
         <v>17</v>
       </c>
@@ -1084,7 +1079,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" s="6" t="s">
         <v>22</v>
       </c>
@@ -1092,10 +1087,10 @@
         <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
       <c r="A51" s="6" t="s">
         <v>22</v>
       </c>
@@ -1103,10 +1098,10 @@
         <v>2</v>
       </c>
       <c r="C51" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
       <c r="A52" s="6" t="s">
         <v>22</v>
       </c>
@@ -1114,10 +1109,10 @@
         <v>3</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" s="6" t="s">
         <v>23</v>
       </c>
@@ -1125,10 +1120,10 @@
         <v>1</v>
       </c>
       <c r="C54" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" s="6" t="s">
         <v>23</v>
       </c>
@@ -1136,10 +1131,10 @@
         <v>2</v>
       </c>
       <c r="C55" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" s="6" t="s">
         <v>23</v>
       </c>
@@ -1147,10 +1142,10 @@
         <v>3</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
       <c r="A58" s="6" t="s">
         <v>24</v>
       </c>
@@ -1161,7 +1156,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3">
       <c r="A59" s="6" t="s">
         <v>24</v>
       </c>
@@ -1172,7 +1167,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60" s="6" t="s">
         <v>24</v>
       </c>
@@ -1183,7 +1178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3">
       <c r="A61" s="6" t="s">
         <v>24</v>
       </c>
@@ -1191,10 +1186,10 @@
         <v>4</v>
       </c>
       <c r="C61" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
       <c r="A62" s="6" t="s">
         <v>24</v>
       </c>
@@ -1202,10 +1197,10 @@
         <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64" s="6" t="s">
         <v>25</v>
       </c>
@@ -1216,7 +1211,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3">
       <c r="A65" s="6" t="s">
         <v>25</v>
       </c>
@@ -1227,7 +1222,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3">
       <c r="A66" s="6" t="s">
         <v>25</v>
       </c>
@@ -1238,7 +1233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3">
       <c r="A67" s="6" t="s">
         <v>25</v>
       </c>
@@ -1246,10 +1241,10 @@
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" s="6" t="s">
         <v>25</v>
       </c>
@@ -1257,30 +1252,30 @@
         <v>5</v>
       </c>
       <c r="C68" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3">
       <c r="A71" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3">
       <c r="A73" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3">
       <c r="A74" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3">
       <c r="A76" s="6" t="s">
         <v>28</v>
       </c>
@@ -1291,7 +1286,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3">
       <c r="A77" s="6" t="s">
         <v>28</v>
       </c>
@@ -1299,10 +1294,10 @@
         <v>2</v>
       </c>
       <c r="C77" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
       <c r="A78" s="6" t="s">
         <v>28</v>
       </c>
@@ -1310,25 +1305,43 @@
         <v>3</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
       <c r="A80" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B80" s="4">
+        <v>1</v>
+      </c>
+      <c r="C80" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
       <c r="A81" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B81" s="4">
+        <v>2</v>
+      </c>
+      <c r="C81" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
       <c r="A82" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B82" s="4">
+        <v>3</v>
+      </c>
+      <c r="C82" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
       <c r="A84" s="6" t="s">
         <v>30</v>
       </c>
@@ -1339,7 +1352,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3">
       <c r="A85" s="6" t="s">
         <v>30</v>
       </c>
@@ -1347,10 +1360,10 @@
         <v>2</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
       <c r="A87" s="6" t="s">
         <v>31</v>
       </c>
@@ -1358,15 +1371,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3">
       <c r="A88" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
       <c r="A90" s="7" t="s">
         <v>32</v>
       </c>
@@ -1374,7 +1387,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3">
       <c r="A91" s="7" t="s">
         <v>32</v>
       </c>
@@ -1382,20 +1395,20 @@
         <v>47</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3">
       <c r="A92" s="7" t="s">
         <v>32</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
       <c r="A94" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3">
       <c r="A96" s="6" t="s">
         <v>34</v>
       </c>
@@ -1403,7 +1416,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3">
       <c r="A98" s="6" t="s">
         <v>18</v>
       </c>
@@ -1414,7 +1427,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3">
       <c r="A99" s="6" t="s">
         <v>18</v>
       </c>
@@ -1425,7 +1438,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3">
       <c r="A100" s="6" t="s">
         <v>18</v>
       </c>
@@ -1436,7 +1449,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3">
       <c r="A101" s="6" t="s">
         <v>18</v>
       </c>
@@ -1447,7 +1460,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3">
       <c r="A103" s="6" t="s">
         <v>35</v>
       </c>
@@ -1458,7 +1471,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3">
       <c r="A104" s="6" t="s">
         <v>35</v>
       </c>
@@ -1469,7 +1482,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3">
       <c r="A106" s="6" t="s">
         <v>36</v>
       </c>
@@ -1477,7 +1490,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3">
       <c r="A107" s="6" t="s">
         <v>36</v>
       </c>
@@ -1485,7 +1498,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3">
       <c r="A108" s="6" t="s">
         <v>36</v>
       </c>
@@ -1493,7 +1506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3">
       <c r="A109" s="6" t="s">
         <v>36</v>
       </c>
@@ -1501,7 +1514,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3">
       <c r="A110" s="6" t="s">
         <v>36</v>
       </c>
@@ -1509,7 +1522,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3">
       <c r="A111" s="6" t="s">
         <v>36</v>
       </c>
@@ -1517,7 +1530,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3">
       <c r="A112" s="6" t="s">
         <v>36</v>
       </c>
@@ -1525,7 +1538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3">
       <c r="A113" s="6" t="s">
         <v>36</v>
       </c>
@@ -1533,7 +1546,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3">
       <c r="A114" s="6" t="s">
         <v>36</v>
       </c>
@@ -1541,7 +1554,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3">
       <c r="A115" s="6" t="s">
         <v>36</v>
       </c>
@@ -1549,7 +1562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3">
       <c r="A117" s="6" t="s">
         <v>37</v>
       </c>
@@ -1560,7 +1573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3">
       <c r="A118" s="6" t="s">
         <v>37</v>
       </c>
@@ -1571,7 +1584,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3">
       <c r="A119" s="6" t="s">
         <v>37</v>
       </c>
@@ -1582,7 +1595,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3">
       <c r="A120" s="6" t="s">
         <v>37</v>
       </c>
@@ -1593,7 +1606,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3">
       <c r="A121" s="6" t="s">
         <v>37</v>
       </c>
@@ -1604,7 +1617,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3">
       <c r="A123" s="6" t="s">
         <v>38</v>
       </c>
@@ -1615,7 +1628,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3">
       <c r="A124" s="6" t="s">
         <v>38</v>
       </c>
@@ -1626,7 +1639,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3">
       <c r="A125" s="6" t="s">
         <v>38</v>
       </c>
@@ -1637,7 +1650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3">
       <c r="A126" s="6" t="s">
         <v>38</v>
       </c>
@@ -1648,7 +1661,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3">
       <c r="A127" s="6" t="s">
         <v>38</v>
       </c>
@@ -1659,7 +1672,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3">
       <c r="A129" s="6" t="s">
         <v>39</v>
       </c>
@@ -1670,7 +1683,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3">
       <c r="A130" s="6" t="s">
         <v>39</v>
       </c>
@@ -1681,7 +1694,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3">
       <c r="A131" s="6" t="s">
         <v>39</v>
       </c>
@@ -1692,7 +1705,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3">
       <c r="A132" s="6" t="s">
         <v>39</v>
       </c>
@@ -1703,7 +1716,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3">
       <c r="A133" s="6" t="s">
         <v>39</v>
       </c>
@@ -1714,7 +1727,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3">
       <c r="A135" s="6" t="s">
         <v>40</v>
       </c>
@@ -1725,7 +1738,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3">
       <c r="A136" s="6" t="s">
         <v>40</v>
       </c>
@@ -1736,7 +1749,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3">
       <c r="A137" s="6" t="s">
         <v>40</v>
       </c>
@@ -1747,7 +1760,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3">
       <c r="A138" s="6" t="s">
         <v>40</v>
       </c>
@@ -1758,7 +1771,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3">
       <c r="A139" s="6" t="s">
         <v>40</v>
       </c>
@@ -1769,7 +1782,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3">
       <c r="A141" s="6" t="s">
         <v>41</v>
       </c>
@@ -1780,7 +1793,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3">
       <c r="A142" s="6" t="s">
         <v>41</v>
       </c>
@@ -1791,7 +1804,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3">
       <c r="A143" s="6" t="s">
         <v>41</v>
       </c>
@@ -1802,7 +1815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3">
       <c r="A144" s="6" t="s">
         <v>41</v>
       </c>
@@ -1813,7 +1826,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3">
       <c r="A145" s="6" t="s">
         <v>41</v>
       </c>
@@ -1824,7 +1837,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3">
       <c r="A147" s="6" t="s">
         <v>42</v>
       </c>
@@ -1835,7 +1848,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3">
       <c r="A148" s="6" t="s">
         <v>42</v>
       </c>
@@ -1846,7 +1859,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3">
       <c r="A149" s="6" t="s">
         <v>42</v>
       </c>
@@ -1857,7 +1870,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3">
       <c r="A150" s="6" t="s">
         <v>42</v>
       </c>
@@ -1868,7 +1881,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3">
       <c r="A151" s="6" t="s">
         <v>42</v>
       </c>
@@ -1881,7 +1894,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Fix naming: "+3.3V_xxx" -> "+3V3_xxx". Add ESTOP signals. Add ABS_ prefixes to some signals.
</commit_message>
<xml_diff>
--- a/Wire Harness/Connector Netlist.xlsx
+++ b/Wire Harness/Connector Netlist.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franklin.320\Wiring Harness\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abk/Dropbox/Documents/OSU/Buckeye Current/Design/Electrical Hardware/Wiring diagrams/Wire Harness/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" tabRatio="500"/>
+    <workbookView xWindow="1920" yWindow="1740" windowWidth="28780" windowHeight="15680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="76">
   <si>
     <t>Connector</t>
   </si>
@@ -122,27 +122,6 @@
     <t>Pin #</t>
   </si>
   <si>
-    <t>GND_FST</t>
-  </si>
-  <si>
-    <t>GND_ST</t>
-  </si>
-  <si>
-    <t>GND_RST</t>
-  </si>
-  <si>
-    <t>GND_MIP</t>
-  </si>
-  <si>
-    <t>GND_AP</t>
-  </si>
-  <si>
-    <t>GND_FTT</t>
-  </si>
-  <si>
-    <t>GND_RTT</t>
-  </si>
-  <si>
     <t>+3.3V</t>
   </si>
   <si>
@@ -191,72 +170,27 @@
     <t>THRTL_POS_RCTL</t>
   </si>
   <si>
-    <t>GND_F1-3</t>
-  </si>
-  <si>
-    <t>GND_F4-6</t>
-  </si>
-  <si>
-    <t>GND_NM</t>
-  </si>
-  <si>
-    <t>GND_IMU</t>
-  </si>
-  <si>
-    <t>+3.3V_MCN1</t>
-  </si>
-  <si>
-    <t>+3.3V_MCN2</t>
-  </si>
-  <si>
     <t>FLOW_MTRLOOP_MCN2 (White)</t>
   </si>
   <si>
     <t>FLOW_MCTLLOOP_MCN2 (White)</t>
   </si>
   <si>
-    <t>+3.3V_THRTLE_POS_RCTL</t>
-  </si>
-  <si>
-    <t>WSP_R</t>
-  </si>
-  <si>
-    <t>WSS_F</t>
-  </si>
-  <si>
-    <t>WSS_R</t>
-  </si>
-  <si>
-    <t>WSP_F</t>
-  </si>
-  <si>
     <t>CAN_A_L</t>
   </si>
   <si>
     <t>CAN_A_H</t>
   </si>
   <si>
-    <t>WAKE_UP_IN</t>
-  </si>
-  <si>
     <t>CAN_2_L</t>
   </si>
   <si>
     <t>CAN_2_H</t>
   </si>
   <si>
-    <t>GND_ECU</t>
-  </si>
-  <si>
     <t>+12V_SYS</t>
   </si>
   <si>
-    <t>GND_CP_MTR</t>
-  </si>
-  <si>
-    <t>GND_CP_MCTL</t>
-  </si>
-  <si>
     <t>+12V_AUX</t>
   </si>
   <si>
@@ -266,22 +200,58 @@
     <t>+5V_MCN3</t>
   </si>
   <si>
-    <t>+5V_MCN2 (Red)</t>
-  </si>
-  <si>
-    <t>GND_CFR1 (Black)</t>
-  </si>
-  <si>
-    <t>GND_CFR2 (Black)</t>
-  </si>
-  <si>
     <t>CN-011</t>
   </si>
   <si>
-    <t>ESTOP</t>
-  </si>
-  <si>
     <t>CN-023</t>
+  </si>
+  <si>
+    <t>+3V3_MCN1</t>
+  </si>
+  <si>
+    <t>GND_MCN1</t>
+  </si>
+  <si>
+    <t>+3V3_MCN2</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>GND_MCN2</t>
+  </si>
+  <si>
+    <t>+5V_MCN2</t>
+  </si>
+  <si>
+    <t>GND_MCN3</t>
+  </si>
+  <si>
+    <t>+3V3_THRTLE_POS_RCTL</t>
+  </si>
+  <si>
+    <t>+12V_ESTOP</t>
+  </si>
+  <si>
+    <t>+12V_NOISE</t>
+  </si>
+  <si>
+    <t>ABS_WSS_R</t>
+  </si>
+  <si>
+    <t>ABS_WSP_F</t>
+  </si>
+  <si>
+    <t>ABS_WAKE_UP</t>
+  </si>
+  <si>
+    <t>ABS_WSP_R</t>
+  </si>
+  <si>
+    <t>ABS_WSS_F</t>
   </si>
 </sst>
 </file>
@@ -333,12 +303,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -363,7 +339,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -391,6 +367,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -745,16 +729,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C142"/>
+  <dimension ref="A1:D143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" style="6"/>
-    <col min="2" max="2" width="6.125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="33" customWidth="1"/>
   </cols>
   <sheetData>
@@ -769,7 +753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -777,10 +761,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
@@ -788,10 +772,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -799,10 +783,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -813,7 +797,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
@@ -824,7 +808,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
@@ -832,10 +816,10 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -843,10 +827,10 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>4</v>
       </c>
@@ -854,10 +838,10 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>4</v>
       </c>
@@ -868,7 +852,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>4</v>
       </c>
@@ -879,7 +863,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>5</v>
       </c>
@@ -887,10 +871,10 @@
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
@@ -898,10 +882,10 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>5</v>
       </c>
@@ -909,10 +893,10 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>5</v>
       </c>
@@ -923,7 +907,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>5</v>
       </c>
@@ -934,7 +918,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
         <v>6</v>
       </c>
@@ -942,10 +926,10 @@
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
         <v>6</v>
       </c>
@@ -953,10 +937,10 @@
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
         <v>7</v>
       </c>
@@ -964,10 +948,10 @@
         <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
         <v>7</v>
       </c>
@@ -975,10 +959,10 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
         <v>7</v>
       </c>
@@ -986,10 +970,10 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
         <v>7</v>
       </c>
@@ -1000,7 +984,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
         <v>7</v>
       </c>
@@ -1011,7 +995,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>8</v>
       </c>
@@ -1019,10 +1003,10 @@
         <v>1</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
         <v>8</v>
       </c>
@@ -1030,10 +1014,10 @@
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>8</v>
       </c>
@@ -1041,10 +1025,10 @@
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>8</v>
       </c>
@@ -1055,7 +1039,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>8</v>
       </c>
@@ -1066,7 +1050,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>9</v>
       </c>
@@ -1074,10 +1058,10 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>9</v>
       </c>
@@ -1085,10 +1069,10 @@
         <v>2</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
         <v>10</v>
       </c>
@@ -1096,10 +1080,10 @@
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
         <v>10</v>
       </c>
@@ -1107,10 +1091,10 @@
         <v>2</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
         <v>11</v>
       </c>
@@ -1118,10 +1102,10 @@
         <v>1</v>
       </c>
       <c r="C41" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
         <v>11</v>
       </c>
@@ -1129,10 +1113,10 @@
         <v>2</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
         <v>12</v>
       </c>
@@ -1140,10 +1124,10 @@
         <v>1</v>
       </c>
       <c r="C44" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
         <v>12</v>
       </c>
@@ -1151,43 +1135,49 @@
         <v>2</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="B47" s="4">
         <v>1</v>
       </c>
       <c r="C47" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="B48" s="4">
         <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D48" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="B49" s="4">
         <v>3</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="D49" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
         <v>14</v>
       </c>
@@ -1195,10 +1185,10 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
         <v>14</v>
       </c>
@@ -1206,10 +1196,13 @@
         <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="D52" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
         <v>14</v>
       </c>
@@ -1217,15 +1210,18 @@
         <v>3</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="D53" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="8"/>
       <c r="B54" s="9"/>
       <c r="C54" s="10"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
         <v>15</v>
       </c>
@@ -1233,10 +1229,10 @@
         <v>1</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
         <v>15</v>
       </c>
@@ -1244,10 +1240,10 @@
         <v>2</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
         <v>15</v>
       </c>
@@ -1255,10 +1251,10 @@
         <v>3</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
         <v>15</v>
       </c>
@@ -1269,7 +1265,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
         <v>15</v>
       </c>
@@ -1280,12 +1276,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="8"/>
       <c r="B60" s="9"/>
       <c r="C60" s="10"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
         <v>16</v>
       </c>
@@ -1293,10 +1289,10 @@
         <v>1</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="8" t="s">
         <v>16</v>
       </c>
@@ -1304,10 +1300,10 @@
         <v>2</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="8" t="s">
         <v>16</v>
       </c>
@@ -1315,10 +1311,10 @@
         <v>3</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="8" t="s">
         <v>16</v>
       </c>
@@ -1329,7 +1325,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="8" t="s">
         <v>16</v>
       </c>
@@ -1340,12 +1336,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="8"/>
       <c r="B66" s="9"/>
       <c r="C66" s="10"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="8" t="s">
         <v>17</v>
       </c>
@@ -1353,10 +1349,10 @@
         <v>1</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="8" t="s">
         <v>17</v>
       </c>
@@ -1364,42 +1360,42 @@
         <v>2</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="8"/>
       <c r="B69" s="9"/>
       <c r="C69" s="10"/>
     </row>
-    <row r="70" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="8" t="s">
+    <row r="70" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B70" s="9">
-        <v>1</v>
-      </c>
-      <c r="C70" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="8" t="s">
+      <c r="B70" s="14">
+        <v>1</v>
+      </c>
+      <c r="C70" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B71" s="9">
-        <v>2</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="14">
+        <v>2</v>
+      </c>
+      <c r="C71" s="16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="8"/>
       <c r="B72" s="9"/>
       <c r="C72" s="10"/>
     </row>
-    <row r="73" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="8" t="s">
         <v>19</v>
       </c>
@@ -1407,10 +1403,10 @@
         <v>1</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="8" t="s">
         <v>19</v>
       </c>
@@ -1421,7 +1417,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="8" t="s">
         <v>19</v>
       </c>
@@ -1429,15 +1425,15 @@
         <v>3</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="8"/>
       <c r="B76" s="9"/>
       <c r="C76" s="10"/>
     </row>
-    <row r="77" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A77" s="8" t="s">
         <v>20</v>
       </c>
@@ -1445,10 +1441,10 @@
         <v>1</v>
       </c>
       <c r="C77" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="8" t="s">
         <v>20</v>
       </c>
@@ -1459,7 +1455,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="8" t="s">
         <v>20</v>
       </c>
@@ -1467,15 +1463,15 @@
         <v>3</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="8"/>
       <c r="B80" s="9"/>
       <c r="C80" s="10"/>
     </row>
-    <row r="81" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="8" t="s">
         <v>21</v>
       </c>
@@ -1483,10 +1479,10 @@
         <v>1</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="8" t="s">
         <v>21</v>
       </c>
@@ -1494,15 +1490,15 @@
         <v>2</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="8"/>
       <c r="B83" s="9"/>
       <c r="C83" s="10"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="8" t="s">
         <v>22</v>
       </c>
@@ -1510,10 +1506,10 @@
         <v>1</v>
       </c>
       <c r="C84" s="10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="8" t="s">
         <v>22</v>
       </c>
@@ -1521,15 +1517,15 @@
         <v>2</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="8"/>
       <c r="B86" s="9"/>
       <c r="C86" s="10"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="12" t="s">
         <v>23</v>
       </c>
@@ -1537,10 +1533,10 @@
         <v>1</v>
       </c>
       <c r="C87" s="10" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="12" t="s">
         <v>23</v>
       </c>
@@ -1548,556 +1544,557 @@
         <v>3</v>
       </c>
       <c r="C88" s="11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="8"/>
       <c r="B89" s="9"/>
       <c r="C89" s="10"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="12" t="s">
         <v>24</v>
       </c>
       <c r="B90" s="4">
         <v>1</v>
       </c>
-      <c r="C90" s="10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B92" s="9"/>
-      <c r="C92" s="10" t="s">
+      <c r="C90" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="12"/>
+      <c r="C91" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B93" s="9"/>
+      <c r="C93" s="10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="8"/>
-      <c r="B93" s="9"/>
-      <c r="C93" s="10"/>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B94" s="9">
-        <v>1</v>
-      </c>
-      <c r="C94" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="8"/>
+      <c r="B94" s="9"/>
+      <c r="C94" s="10"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B95" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B96" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="8" t="s">
         <v>25</v>
       </c>
       <c r="B97" s="9">
+        <v>3</v>
+      </c>
+      <c r="C97" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B98" s="9">
         <v>4</v>
       </c>
-      <c r="C97" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="8"/>
-      <c r="B98" s="9"/>
-      <c r="C98" s="10"/>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B99" s="9">
-        <v>1</v>
-      </c>
-      <c r="C99" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C98" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="8"/>
+      <c r="B99" s="9"/>
+      <c r="C99" s="10"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B100" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B101" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C101" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B102" s="9">
-        <v>4</v>
-      </c>
-      <c r="C102" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="C102" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B103" s="9">
+        <v>4</v>
+      </c>
+      <c r="C103" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B104" s="9">
         <v>5</v>
       </c>
-      <c r="C103" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="8"/>
-      <c r="B104" s="9"/>
-      <c r="C104" s="10"/>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B105" s="9">
-        <v>1</v>
-      </c>
-      <c r="C105" s="11" t="s">
+      <c r="C104" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="8"/>
+      <c r="B105" s="9"/>
+      <c r="C105" s="10"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B106" s="9">
+        <v>1</v>
+      </c>
+      <c r="C106" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B107" s="9">
+        <v>2</v>
+      </c>
+      <c r="C107" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B108" s="9">
+        <v>3</v>
+      </c>
+      <c r="C108" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B109" s="9">
+        <v>4</v>
+      </c>
+      <c r="C109" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B110" s="9">
+        <v>5</v>
+      </c>
+      <c r="C110" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B111" s="9">
+        <v>6</v>
+      </c>
+      <c r="C111" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B112" s="9">
+        <v>7</v>
+      </c>
+      <c r="C112" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B113" s="9">
+        <v>8</v>
+      </c>
+      <c r="C113" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B114" s="9">
+        <v>9</v>
+      </c>
+      <c r="C114" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B115" s="9">
+        <v>10</v>
+      </c>
+      <c r="C115" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B116" s="9">
+        <v>11</v>
+      </c>
+      <c r="C116" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B117" s="9">
+        <v>12</v>
+      </c>
+      <c r="C117" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B118" s="9">
+        <v>13</v>
+      </c>
+      <c r="C118" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B119" s="9">
+        <v>14</v>
+      </c>
+      <c r="C119" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B120" s="9">
+        <v>15</v>
+      </c>
+      <c r="C120" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B121" s="9">
+        <v>16</v>
+      </c>
+      <c r="C121" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B122" s="9">
+        <v>17</v>
+      </c>
+      <c r="C122" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B123" s="9">
+        <v>18</v>
+      </c>
+      <c r="C123" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B124" s="9">
+        <v>19</v>
+      </c>
+      <c r="C124" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B125" s="9">
+        <v>20</v>
+      </c>
+      <c r="C125" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B126" s="9">
+        <v>21</v>
+      </c>
+      <c r="C126" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B127" s="9">
+        <v>22</v>
+      </c>
+      <c r="C127" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B128" s="9">
+        <v>23</v>
+      </c>
+      <c r="C128" s="10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B106" s="9">
-        <v>2</v>
-      </c>
-      <c r="C106" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B107" s="9">
-        <v>3</v>
-      </c>
-      <c r="C107" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B108" s="9">
-        <v>4</v>
-      </c>
-      <c r="C108" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B109" s="9">
-        <v>5</v>
-      </c>
-      <c r="C109" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B110" s="9">
-        <v>6</v>
-      </c>
-      <c r="C110" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B111" s="9">
-        <v>7</v>
-      </c>
-      <c r="C111" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B112" s="9">
-        <v>8</v>
-      </c>
-      <c r="C112" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B113" s="9">
-        <v>9</v>
-      </c>
-      <c r="C113" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B114" s="9">
-        <v>10</v>
-      </c>
-      <c r="C114" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B115" s="9">
-        <v>11</v>
-      </c>
-      <c r="C115" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B116" s="9">
-        <v>12</v>
-      </c>
-      <c r="C116" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B117" s="9">
-        <v>13</v>
-      </c>
-      <c r="C117" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B118" s="9">
-        <v>14</v>
-      </c>
-      <c r="C118" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B119" s="9">
-        <v>15</v>
-      </c>
-      <c r="C119" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B120" s="9">
-        <v>16</v>
-      </c>
-      <c r="C120" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B121" s="9">
-        <v>17</v>
-      </c>
-      <c r="C121" s="11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B122" s="9">
-        <v>18</v>
-      </c>
-      <c r="C122" s="10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B123" s="9">
-        <v>19</v>
-      </c>
-      <c r="C123" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B124" s="9">
-        <v>20</v>
-      </c>
-      <c r="C124" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B125" s="9">
-        <v>21</v>
-      </c>
-      <c r="C125" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B126" s="9">
-        <v>22</v>
-      </c>
-      <c r="C126" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B127" s="9">
-        <v>23</v>
-      </c>
-      <c r="C127" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B128" s="9">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B129" s="9">
         <v>24</v>
       </c>
-      <c r="C128" s="11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B129" s="9">
+      <c r="C129" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B130" s="9">
         <v>25</v>
       </c>
-      <c r="C129" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B130" s="9">
-        <v>26</v>
-      </c>
-      <c r="C130" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="8"/>
-      <c r="B131" s="9"/>
-      <c r="C131" s="10"/>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B132" s="9">
-        <v>1</v>
-      </c>
-      <c r="C132" s="11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C130" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B131" s="9">
+        <v>26</v>
+      </c>
+      <c r="C131" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" s="8"/>
+      <c r="B132" s="9"/>
+      <c r="C132" s="10"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B133" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C133" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B134" s="9">
-        <v>3</v>
-      </c>
-      <c r="C134" s="10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C134" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="8" t="s">
         <v>27</v>
       </c>
       <c r="B135" s="9">
+        <v>3</v>
+      </c>
+      <c r="C135" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B136" s="9">
         <v>4</v>
       </c>
-      <c r="C135" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="6" t="s">
+      <c r="C136" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B136" s="4">
+      <c r="B137" s="4">
         <v>5</v>
       </c>
-      <c r="C136" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A138" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B138" s="4">
-        <v>1</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C137" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B139" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B140" s="4">
-        <v>3</v>
-      </c>
-      <c r="C140" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B141" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C141" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B142" s="4">
+        <v>4</v>
+      </c>
+      <c r="C142" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B143" s="4">
         <v>5</v>
       </c>
-      <c r="C142" t="s">
-        <v>68</v>
+      <c r="C143" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>